<commit_message>
Bonus exercise plus small improvements
</commit_message>
<xml_diff>
--- a/teched2025-CA262-Results.xlsx
+++ b/teched2025-CA262-Results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAPDevelop\com.sap.teched\teched2025-CA262\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I521046\teched2025-CA262\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9487F4-052D-4800-B9CE-3FCA589F3D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3672CA1B-FA55-4948-8E99-AF47D45E07A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{90680149-6A1A-4992-B9DA-B35947F123DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{90680149-6A1A-4992-B9DA-B35947F123DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Disabled Cache</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Number of requests</t>
   </si>
   <si>
-    <t>Bytes transferred</t>
-  </si>
-  <si>
-    <t>Bytes loaded</t>
-  </si>
-  <si>
-    <t>Finish time</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -119,26 +110,44 @@
     <t>Total number of requests for the initial load.</t>
   </si>
   <si>
-    <t>Enter your measurements here. Use a comma as the decimal separator.</t>
-  </si>
-  <si>
-    <t>Amount of uncompressed data for the initial load</t>
-  </si>
-  <si>
-    <t>Requests fetched from the server for the initial load</t>
-  </si>
-  <si>
-    <t>Requests served from cache for the initial load</t>
-  </si>
-  <si>
-    <t>Requests resulted in a 304 for the initial load</t>
-  </si>
-  <si>
     <t>Exercise 1.3</t>
   </si>
   <si>
+    <t>Amount of transferred data for the initial load</t>
+  </si>
+  <si>
+    <t>Amount of transferred data for the intial load</t>
+  </si>
+  <si>
+    <t>Number of requests served from cache for the initial load</t>
+  </si>
+  <si>
+    <t>Number of requests fetched from the server for the initial load</t>
+  </si>
+  <si>
+    <t>Number of requests resulted in a 304 for the initial load</t>
+  </si>
+  <si>
+    <t>Size of loaded resources for the initial load</t>
+  </si>
+  <si>
+    <t>Finish time (at least 5 iterations)</t>
+  </si>
+  <si>
+    <t>Build with MDC (optional)</t>
+  </si>
+  <si>
+    <t>Build with MDC and FL (optional)</t>
+  </si>
+  <si>
+    <t>Build with MDC, FL and F (opt.)</t>
+  </si>
+  <si>
+    <t>Enter your measurements here. Make sure to use the correct decimal separator and to not include units. They are automatically set.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Enter your measurements here. Use a comma as the decimal separator. The average of the </t>
+      <t xml:space="preserve">The average of the </t>
     </r>
     <r>
       <rPr>
@@ -157,8 +166,14 @@
         <rFont val="72 Brand"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> will be automatically updated when entering data for the iterations.</t>
+      <t xml:space="preserve"> will be automatically updated when entering data for the iterations. Remember to use the correct decimal separator and to not include units.</t>
     </r>
+  </si>
+  <si>
+    <t>Data transferred</t>
+  </si>
+  <si>
+    <t>Resources loaded</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1F2328"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="72 Brand"/>
       <family val="2"/>
     </font>
@@ -328,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -363,34 +378,8 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -419,49 +408,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" indent="10"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -475,10 +501,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD1EFFF"/>
       <color rgb="FF002A86"/>
       <color rgb="FFEAECEE"/>
       <color rgb="FF89D1FF"/>
-      <color rgb="FFD1EFFF"/>
       <color rgb="FF00144A"/>
       <color rgb="FFE8F7FC"/>
       <color rgb="FFE88CD6"/>
@@ -815,358 +841,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA9ED4D-C24A-470D-9F5C-737C5A215A21}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="17" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="12" customWidth="1"/>
+    <col min="3" max="17" width="11.7109375" style="12" customWidth="1"/>
     <col min="18" max="24" width="0" hidden="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-    </row>
-    <row r="2" spans="1:24" s="35" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:24" s="23" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22"/>
+      <c r="B2" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+    </row>
+    <row r="3" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-    </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="39" t="s">
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="Q4" s="13"/>
+    </row>
+    <row r="5" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="Q5" s="12"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="14"/>
+      <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6" s="47"/>
       <c r="K6" s="47"/>
-      <c r="L6" s="25"/>
-      <c r="Q6" s="12"/>
+      <c r="L6" s="21"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="48" t="s">
         <v>29</v>
       </c>
       <c r="J7" s="48"/>
       <c r="K7" s="48"/>
-      <c r="L7" s="32"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="2"/>
+      <c r="L7" s="14"/>
+      <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="47" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J8" s="47"/>
       <c r="K8" s="47"/>
-      <c r="L8" s="25"/>
-      <c r="Q8" s="12"/>
+      <c r="L8" s="29"/>
+      <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="48" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J9" s="48"/>
       <c r="K9" s="48"/>
-      <c r="L9" s="31"/>
-      <c r="Q9" s="12"/>
+      <c r="L9" s="30"/>
+      <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="24"/>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-    </row>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="28"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
+      <c r="B12" s="24" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
+      <c r="B13" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="G17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="H17" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="15" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="J17" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="K17" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="L17" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="M17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="N17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="O17" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="P17" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="14" t="s">
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="O17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="P17" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
-        <v>17</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="17">
+      <c r="F18" s="36">
         <f>IFERROR(AVERAGE(G18:P18),0)</f>
         <v>0</v>
       </c>
@@ -1182,13 +1172,13 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>18</v>
+      <c r="B19" s="37" t="s">
+        <v>15</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="19">
+      <c r="F19" s="38">
         <f t="shared" ref="F19:F22" si="0">IFERROR(AVERAGE(G19:P19),0)</f>
         <v>0</v>
       </c>
@@ -1204,13 +1194,13 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>19</v>
+      <c r="B20" s="39" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="17">
+      <c r="F20" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1226,13 +1216,13 @@
       <c r="P20" s="11"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>20</v>
+      <c r="B21" s="37" t="s">
+        <v>17</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="19">
+      <c r="F21" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1248,13 +1238,13 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>21</v>
+      <c r="B22" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="17">
+      <c r="F22" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1270,268 +1260,264 @@
       <c r="P22" s="11"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="2:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="2:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+    </row>
+    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="41" t="s">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="G26" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="H26" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
+      <c r="I26" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="O26" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="N27" s="14" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="O27" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="P27" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="36">
+        <f>IFERROR(AVERAGE(G27:P27),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="17">
-        <f>IFERROR(AVERAGE(G28:P28),0)</f>
+      <c r="B28" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="38">
+        <f t="shared" ref="F28:F31" si="1">IFERROR(AVERAGE(G28:P28),0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="19">
-        <f t="shared" ref="F29:F32" si="1">IFERROR(AVERAGE(G29:P29),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="17">
+      <c r="B29" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="19">
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="17">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-    </row>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25"/>
     <row r="33" x14ac:dyDescent="0.25"/>
-    <row r="34" x14ac:dyDescent="0.25"/>
-    <row r="35" x14ac:dyDescent="0.25"/>
-    <row r="36" x14ac:dyDescent="0.25"/>
-    <row r="37" x14ac:dyDescent="0.25"/>
-    <row r="38" x14ac:dyDescent="0.25"/>
-    <row r="39" x14ac:dyDescent="0.25"/>
-    <row r="40" x14ac:dyDescent="0.25"/>
-    <row r="41" x14ac:dyDescent="0.25"/>
-    <row r="42" x14ac:dyDescent="0.25"/>
-    <row r="43" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="18">
-    <mergeCell ref="I2:J2"/>
+  <mergeCells count="19">
+    <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="F26:P26"/>
+    <mergeCell ref="F25:P25"/>
     <mergeCell ref="B13:P13"/>
-    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B2:K2"/>
     <mergeCell ref="F16:P16"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="I8:K8"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please use the correct decimal separator and do not specify any units._x000a_The unit &quot;s&quot; is automatically applied." sqref="G18:P22 G27:P31" xr:uid="{07DD06AE-E8B6-4D28-9192-1E0E8905362B}">
+      <formula1>0</formula1>
+      <formula2>9999</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please enter only whole numbers." sqref="C5 L5:L7 C18:C22 C27:C31" xr:uid="{F6AE6D37-6C52-49C0-9971-A6C350692270}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please use the correct decimal separator and do not specify any units._x000a_The unit &quot;MB&quot; is automatically applied." sqref="C6:C7 L9 D18:E22 E27:E31" xr:uid="{AF22252C-2F42-4D9E-9FEF-232D17E267ED}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please use the correct decimal separator and do not specify any units._x000a_The unit &quot;kB&quot; is automatically applied." sqref="L8" xr:uid="{4DB3C168-577D-41F1-B4D2-0983FDB27F00}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please use the correct decimal separator and do not specify any units._x000a_The unit &quot;s&quot; is automatically applied." sqref="L10 C8" xr:uid="{CECBDEB4-F742-43BF-92D6-AE3BC6EE10E6}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong format" error="Please use the correct decimal separator and do not specify any units._x000a_The unit &quot;kB&quot; is automatically applied." sqref="D27:D31" xr:uid="{C805F6FC-0DBA-42D2-8AE2-062AA2F92996}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>